<commit_message>
minor: rename moq to minimum order qty in excel template for photo quotation
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/lead_items_supplier_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/lead_items_supplier_template.xlsx
@@ -166,7 +166,7 @@
     <t xml:space="preserve">packing_type</t>
   </si>
   <si>
-    <t xml:space="preserve">moq</t>
+    <t xml:space="preserve">minimum_order_qty</t>
   </si>
   <si>
     <t xml:space="preserve">unit_price</t>
@@ -561,9 +561,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>439920</xdr:colOff>
+      <xdr:colOff>439560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>807480</xdr:rowOff>
+      <xdr:rowOff>807120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -577,12 +577,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="19080"/>
-          <a:ext cx="1216440" cy="1226520"/>
+          <a:ext cx="1216080" cy="1226160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -600,10 +600,10 @@
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="B16 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -5731,8 +5731,8 @@
     <mergeCell ref="Q5:X5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5749,10 +5749,10 @@
   <dimension ref="A1:AO25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.8"/>
@@ -6015,7 +6015,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
feat: rearrange columns in photo quotation child table
upload of supplier templat to photo quotation child table
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/lead_items_supplier_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/lead_items_supplier_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lead Items" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t xml:space="preserve">ARTYFETES FACTORY
 ZA DE LA MESNILIERE 
@@ -115,6 +115,9 @@
     <t xml:space="preserve">PO created</t>
   </si>
   <si>
+    <t xml:space="preserve">Lead Item</t>
+  </si>
+  <si>
     <t xml:space="preserve">HEADER</t>
   </si>
   <si>
@@ -124,13 +127,13 @@
     <t xml:space="preserve">SKIP ROWS</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
+    <t xml:space="preserve">supplier_part_no</t>
   </si>
   <si>
     <t xml:space="preserve">item_photo</t>
   </si>
   <si>
-    <t xml:space="preserve">description</t>
+    <t xml:space="preserve">supplier_item_description</t>
   </si>
   <si>
     <t xml:space="preserve">product_material1</t>
@@ -194,6 +197,12 @@
   </si>
   <si>
     <t xml:space="preserve">is_po_created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead Item#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
   </si>
 </sst>
 </file>
@@ -561,9 +570,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>439560</xdr:colOff>
+      <xdr:colOff>439200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>807120</xdr:rowOff>
+      <xdr:rowOff>806760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -577,7 +586,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="19080"/>
-          <a:ext cx="1216080" cy="1226160"/>
+          <a:ext cx="1215720" cy="1225800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -599,11 +608,11 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="B16 A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X9" activeCellId="0" sqref="X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -828,6 +837,9 @@
       </c>
       <c r="X6" s="18" t="s">
         <v>27</v>
+      </c>
+      <c r="Y6" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5746,13 +5758,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO25"/>
+  <dimension ref="A1:AO26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.8"/>
@@ -5761,13 +5773,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5775,7 +5787,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="22" t="n">
         <v>6</v>
@@ -5786,7 +5798,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="22"/>
     </row>
@@ -5795,7 +5807,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="22"/>
     </row>
@@ -5804,7 +5816,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="22"/>
     </row>
@@ -5813,7 +5825,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="22"/>
       <c r="R6" s="16"/>
@@ -5846,7 +5858,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="22"/>
     </row>
@@ -5855,7 +5867,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="22"/>
     </row>
@@ -5864,7 +5876,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="22"/>
     </row>
@@ -5873,7 +5885,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" s="22"/>
     </row>
@@ -5882,7 +5894,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="22"/>
     </row>
@@ -5891,7 +5903,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="22"/>
     </row>
@@ -5900,7 +5912,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="22"/>
     </row>
@@ -5909,7 +5921,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="22"/>
     </row>
@@ -5918,7 +5930,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="22"/>
     </row>
@@ -5927,7 +5939,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="22"/>
     </row>
@@ -5936,7 +5948,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="22"/>
     </row>
@@ -5945,7 +5957,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" s="22"/>
     </row>
@@ -5954,7 +5966,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" s="22"/>
     </row>
@@ -5963,7 +5975,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="22"/>
     </row>
@@ -5972,7 +5984,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" s="22"/>
     </row>
@@ -5981,7 +5993,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="22"/>
     </row>
@@ -5990,7 +6002,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="22"/>
     </row>
@@ -5999,7 +6011,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" s="22"/>
     </row>
@@ -6008,9 +6020,18 @@
         <v>27</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="23"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: add drop down list in photo quotation excel
add certificates required in supplier pq template
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/lead_items_supplier_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/lead_items_supplier_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t xml:space="preserve">ARTYFETES FACTORY
 ZA DE LA MESNILIERE 
@@ -98,6 +98,10 @@
   </si>
   <si>
     <t xml:space="preserve">Special mentions ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificates
+Required ?</t>
   </si>
   <si>
     <t xml:space="preserve">Test Report</t>
@@ -182,6 +186,12 @@
   </si>
   <si>
     <t xml:space="preserve">is_special_mentions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificates required ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_certificates_reqd</t>
   </si>
   <si>
     <t xml:space="preserve">test_report</t>
@@ -570,9 +580,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>439200</xdr:colOff>
+      <xdr:colOff>438840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>806760</xdr:rowOff>
+      <xdr:rowOff>806400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -586,7 +596,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="19080"/>
-          <a:ext cx="1215720" cy="1225800"/>
+          <a:ext cx="1215360" cy="1225440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -608,11 +618,11 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X9" activeCellId="0" sqref="X9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -631,7 +641,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.43"/>
@@ -840,6 +850,9 @@
       </c>
       <c r="Y6" s="18" t="s">
         <v>28</v>
+      </c>
+      <c r="Z6" s="18" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5758,10 +5771,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO26"/>
+  <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5773,13 +5786,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5787,7 +5800,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="22" t="n">
         <v>6</v>
@@ -5798,7 +5811,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="22"/>
     </row>
@@ -5807,7 +5820,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="22"/>
     </row>
@@ -5816,7 +5829,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="22"/>
     </row>
@@ -5825,7 +5838,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="22"/>
       <c r="R6" s="16"/>
@@ -5858,7 +5871,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="22"/>
     </row>
@@ -5867,7 +5880,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="22"/>
     </row>
@@ -5876,7 +5889,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="22"/>
     </row>
@@ -5885,7 +5898,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="22"/>
     </row>
@@ -5894,7 +5907,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="22"/>
     </row>
@@ -5903,7 +5916,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="22"/>
     </row>
@@ -5912,7 +5925,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="22"/>
     </row>
@@ -5921,7 +5934,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="22"/>
     </row>
@@ -5930,7 +5943,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="22"/>
     </row>
@@ -5939,7 +5952,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="22"/>
     </row>
@@ -5948,7 +5961,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="22"/>
     </row>
@@ -5957,7 +5970,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="22"/>
     </row>
@@ -5966,7 +5979,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="22"/>
     </row>
@@ -5975,16 +5988,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="21" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" s="22"/>
     </row>
@@ -5993,7 +6006,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C22" s="22"/>
     </row>
@@ -6002,7 +6015,7 @@
         <v>25</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" s="22"/>
     </row>
@@ -6011,7 +6024,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C24" s="22"/>
     </row>
@@ -6019,19 +6032,28 @@
       <c r="A25" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="23"/>
+      <c r="B25" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="21" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="23"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>